<commit_message>
creation csv pour abstract
</commit_message>
<xml_diff>
--- a/DB/data_base_glendu/Données labo glendu.xlsx
+++ b/DB/data_base_glendu/Données labo glendu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15819\Desktop\TPOP_lou_et_melo_OwO\DB\data_base_glendu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{521C604E-3D53-4559-9A7C-F3CAEE98A924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2CADB0-6011-47D3-93C8-833CC8ED8E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0D81227F-8FEF-4CF9-8A79-3C3D9E04F552}"/>
   </bookViews>
@@ -119,12 +119,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3824,7 +3823,7 @@
   <dimension ref="B2:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
-      <selection activeCell="AB33" sqref="AB33"/>
+      <selection activeCell="J3" sqref="J3:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3835,7 +3834,6 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="2"/>
       <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
@@ -3845,7 +3843,6 @@
         <v>10</v>
       </c>
       <c r="K2" s="1"/>
-      <c r="L2" s="2"/>
       <c r="M2" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>